<commit_message>
static: new program added, menu changed
</commit_message>
<xml_diff>
--- a/static/xlsx/Programlar.xlsx
+++ b/static/xlsx/Programlar.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>İsim</t>
   </si>
@@ -74,6 +74,15 @@
   </si>
   <si>
     <t>https://apply.aspireleaders.org/f/64413a183b5d0038f900087e</t>
+  </si>
+  <si>
+    <t>GDSC Leads</t>
+  </si>
+  <si>
+    <t>14.07.2023</t>
+  </si>
+  <si>
+    <t>https://developers.google.com/community/gdsc/leads</t>
   </si>
 </sst>
 </file>
@@ -81,10 +90,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="21">
@@ -112,16 +121,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -129,21 +169,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -197,52 +222,36 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -257,31 +266,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -293,151 +416,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -448,6 +457,41 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -499,30 +543,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -537,29 +557,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -575,124 +584,124 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1026,7 +1035,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1124,7 +1133,16 @@
       </c>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="4:4">
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="D8" s="6"/>
     </row>
     <row r="9" spans="4:4">

</xml_diff>

<commit_message>
static: imagine program added
</commit_message>
<xml_diff>
--- a/static/xlsx/Programlar.xlsx
+++ b/static/xlsx/Programlar.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>İsim</t>
   </si>
@@ -83,6 +83,15 @@
   </si>
   <si>
     <t>https://developers.google.com/community/gdsc/leads</t>
+  </si>
+  <si>
+    <t>Microsoft Imagine</t>
+  </si>
+  <si>
+    <t>20.11.2022</t>
+  </si>
+  <si>
+    <t>https://bidb.iyte.edu.tr/microsoft-imagine-academy/</t>
   </si>
 </sst>
 </file>
@@ -90,10 +99,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="21">
@@ -129,6 +138,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -137,7 +161,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -145,38 +177,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -190,8 +191,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -213,21 +245,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -236,22 +253,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -266,127 +275,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -398,55 +443,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -457,6 +466,69 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -489,71 +561,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -563,12 +572,12 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -581,85 +590,85 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -668,40 +677,40 @@
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1035,7 +1044,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1145,7 +1154,16 @@
       </c>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="4:4">
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="D9" s="6"/>
     </row>
     <row r="10" spans="4:4">

</xml_diff>

<commit_message>
static: devpaths program added
</commit_message>
<xml_diff>
--- a/static/xlsx/Programlar.xlsx
+++ b/static/xlsx/Programlar.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>İsim</t>
   </si>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t>https://airtable.com/shrjRQI3DjWuGQuyO</t>
+  </si>
+  <si>
+    <t>DevPaths</t>
+  </si>
+  <si>
+    <t>https://kesisenyollar.org/devpaths/</t>
   </si>
 </sst>
 </file>
@@ -118,10 +124,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="m/d/yyyy;@"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -148,9 +154,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -158,6 +193,22 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -165,14 +216,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -186,92 +253,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -293,19 +299,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -317,163 +455,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -487,25 +493,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -529,8 +522,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -560,6 +553,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -576,26 +584,24 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -608,28 +614,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -638,97 +644,97 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1062,7 +1068,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1208,7 +1214,16 @@
       </c>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="4:4">
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D12" s="6"/>
     </row>
     <row r="13" spans="4:4">

</xml_diff>